<commit_message>
update readme, add workbooks
</commit_message>
<xml_diff>
--- a/resources/SIMPLE-1.xlsx
+++ b/resources/SIMPLE-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\kowens\dev\xl-parse-clj\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD8B625-A94D-49EC-A4F8-E58357144BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96D1832-80BE-4112-A1B0-1383224EB829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2736" yWindow="624" windowWidth="15684" windowHeight="11112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2736" yWindow="624" windowWidth="18648" windowHeight="11112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" r:id="rId1"/>
@@ -393,7 +393,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>